<commit_message>
Added a few comments, few clean-ups in the code.
</commit_message>
<xml_diff>
--- a/Test Excel File/Example.xlsx
+++ b/Test Excel File/Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Test Excel File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5845046-938B-4137-8794-CCA057DF93B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C764060E-F6BF-4EE9-B543-E3A7A7DF4EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="-3135" windowWidth="15600" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="41" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>/object1/object2/field11</t>
   </si>
   <si>
-    <t>/field12</t>
-  </si>
-  <si>
     <t>1,2,3</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>/object5/field15</t>
+  </si>
+  <si>
+    <t>/field99</t>
   </si>
 </sst>
 </file>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486EB83C-7ED2-445D-887A-8B2E303F2CB4}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +951,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>11</v>
@@ -968,7 +968,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>11</v>
@@ -1045,7 +1045,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>9</v>
@@ -1056,7 +1056,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>8</v>
@@ -1086,7 +1086,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>8</v>
@@ -1116,7 +1116,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>8</v>
@@ -1131,7 +1131,7 @@
         <v>10</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>8</v>
@@ -1161,7 +1161,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
done but few tweaks need to be done
</commit_message>
<xml_diff>
--- a/Test Excel File/Example.xlsx
+++ b/Test Excel File/Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Test Excel File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F30A8E-B702-4E2F-8A9F-498189F7755E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDCF555-4461-4184-A7BB-9F2E1EC8E904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3315" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="41" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="66">
   <si>
     <t>I/o</t>
   </si>
@@ -179,12 +179,6 @@
     <t>/field99</t>
   </si>
   <si>
-    <t>GGWP (API_NAME)</t>
-  </si>
-  <si>
-    <t>ZOMBIE</t>
-  </si>
-  <si>
     <t>/gg</t>
   </si>
   <si>
@@ -222,6 +216,33 @@
   </si>
   <si>
     <t>/gg/object2/field11</t>
+  </si>
+  <si>
+    <t>GGWP22 (API_NAME)</t>
+  </si>
+  <si>
+    <t>GGWP33(API_NAME)</t>
+  </si>
+  <si>
+    <t>dsfsf(API_NAME)</t>
+  </si>
+  <si>
+    <t>GGWhshshP33(AsdPI_NAME)</t>
+  </si>
+  <si>
+    <t>ZOMBIsdsdsdE22</t>
+  </si>
+  <si>
+    <t>ZOMsdsdBIE22</t>
+  </si>
+  <si>
+    <t>ZOsdsdsdMBIE11</t>
+  </si>
+  <si>
+    <t>ZOMdfsdfBIE22</t>
+  </si>
+  <si>
+    <t>ZOdsfggMBIE22</t>
   </si>
 </sst>
 </file>
@@ -830,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486EB83C-7ED2-445D-887A-8B2E303F2CB4}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:E85"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1228,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B30" s="16"/>
     </row>
@@ -1221,7 +1242,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>14</v>
@@ -1249,7 +1270,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>18</v>
@@ -1264,7 +1285,7 @@
         <v>7</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>8</v>
@@ -1279,7 +1300,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>8</v>
@@ -1294,7 +1315,7 @@
         <v>7</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>8</v>
@@ -1309,7 +1330,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>8</v>
@@ -1324,7 +1345,7 @@
         <v>7</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>19</v>
@@ -1339,7 +1360,7 @@
         <v>7</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>8</v>
@@ -1356,7 +1377,7 @@
         <v>7</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>8</v>
@@ -1373,7 +1394,7 @@
         <v>7</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>8</v>
@@ -1388,7 +1409,7 @@
         <v>7</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>8</v>
@@ -1403,7 +1424,7 @@
         <v>7</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>8</v>
@@ -1418,7 +1439,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>8</v>
@@ -1433,7 +1454,7 @@
         <v>7</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>8</v>
@@ -1567,7 +1588,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B59" s="16"/>
     </row>
@@ -1581,7 +1602,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>14</v>
@@ -1609,7 +1630,7 @@
         <v>7</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>18</v>
@@ -1624,7 +1645,7 @@
         <v>7</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>8</v>
@@ -1639,7 +1660,7 @@
         <v>7</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>8</v>
@@ -1654,7 +1675,7 @@
         <v>7</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>8</v>
@@ -1669,7 +1690,7 @@
         <v>7</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>8</v>
@@ -1684,7 +1705,7 @@
         <v>7</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>19</v>
@@ -1699,7 +1720,7 @@
         <v>7</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>8</v>
@@ -1716,7 +1737,7 @@
         <v>7</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>8</v>
@@ -1733,7 +1754,7 @@
         <v>7</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>8</v>
@@ -1748,7 +1769,7 @@
         <v>7</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>8</v>
@@ -1763,7 +1784,7 @@
         <v>7</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>8</v>
@@ -1778,7 +1799,7 @@
         <v>7</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>8</v>
@@ -1793,7 +1814,7 @@
         <v>7</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>8</v>
@@ -1922,6 +1943,1086 @@
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B89" s="16"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D95" s="11"/>
+      <c r="E95" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="3"/>
+      <c r="E96" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="3"/>
+      <c r="E97" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" s="3"/>
+      <c r="E98" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B99" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" s="3"/>
+      <c r="E99" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D100" s="11"/>
+      <c r="E100" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" s="3"/>
+      <c r="E103" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" s="3"/>
+      <c r="E104" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" s="3"/>
+      <c r="E105" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D106" s="3"/>
+      <c r="E106" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" s="3"/>
+      <c r="E108" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D109" s="11"/>
+      <c r="E109" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B110" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D110" s="3"/>
+      <c r="E110" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D111" s="11"/>
+      <c r="E111" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B112" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112" s="3"/>
+      <c r="E112" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B113" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D113" s="3"/>
+      <c r="E113" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D114" s="11"/>
+      <c r="E114" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" s="3"/>
+      <c r="E115" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B119" s="16"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D125" s="11"/>
+      <c r="E125" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" s="3"/>
+      <c r="E127" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B128" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D128" s="3"/>
+      <c r="E128" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" s="3"/>
+      <c r="E129" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C130" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D130" s="11"/>
+      <c r="E130" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B132" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B133" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D133" s="3"/>
+      <c r="E133" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B134" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D134" s="3"/>
+      <c r="E134" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B135" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D135" s="3"/>
+      <c r="E135" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B136" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D136" s="3"/>
+      <c r="E136" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B137" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B138" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" s="3"/>
+      <c r="E138" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B139" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C139" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D139" s="11"/>
+      <c r="E139" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B140" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D140" s="3"/>
+      <c r="E140" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B141" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C141" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D141" s="11"/>
+      <c r="E141" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B142" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" s="3"/>
+      <c r="E142" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B143" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" s="3"/>
+      <c r="E143" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C144" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D144" s="11"/>
+      <c r="E144" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B145" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D145" s="3"/>
+      <c r="E145" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B150" s="16"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B156" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C156" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D156" s="11"/>
+      <c r="E156" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B157" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D157" s="3"/>
+      <c r="E157" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B158" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D158" s="3"/>
+      <c r="E158" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B159" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D159" s="3"/>
+      <c r="E159" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B160" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D160" s="3"/>
+      <c r="E160" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B161" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C161" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D161" s="11"/>
+      <c r="E161" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B162" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E162" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B163" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E163" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D164" s="3"/>
+      <c r="E164" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B165" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D165" s="3"/>
+      <c r="E165" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B166" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D166" s="3"/>
+      <c r="E166" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B167" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D167" s="3"/>
+      <c r="E167" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B168" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E168" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B169" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D169" s="3"/>
+      <c r="E169" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B170" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C170" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D170" s="11"/>
+      <c r="E170" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B171" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D171" s="3"/>
+      <c r="E171" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B172" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C172" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D172" s="11"/>
+      <c r="E172" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B173" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D173" s="3"/>
+      <c r="E173" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B174" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D174" s="3"/>
+      <c r="E174" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B175" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C175" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D175" s="11"/>
+      <c r="E175" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B176" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D176" s="3"/>
+      <c r="E176" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>